<commit_message>
further improved analysis. Data sets are ready
</commit_message>
<xml_diff>
--- a/code/results/userStudies_exp1_results/analysis_subjective.xlsx
+++ b/code/results/userStudies_exp1_results/analysis_subjective.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="35"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="995" firstSheet="0" activeTab="35"/>
   </bookViews>
   <sheets>
     <sheet name="task_tedious" sheetId="1" state="visible" r:id="rId2"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="75">
   <si>
     <t xml:space="preserve">The tasks were tedious (boring and monotonous)</t>
   </si>
@@ -274,10 +274,10 @@
     <t xml:space="preserve">Selection</t>
   </si>
   <si>
-    <t xml:space="preserve">%10</t>
+    <t xml:space="preserve">%30.77</t>
   </si>
   <si>
-    <t xml:space="preserve">%90</t>
+    <t xml:space="preserve">%69.23</t>
   </si>
   <si>
     <t xml:space="preserve">Which robot was learning and adapting better to your assistance needs?</t>
@@ -296,6 +296,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -316,12 +317,14 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -372,7 +375,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -417,6 +420,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -438,16 +445,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -848,6 +852,29 @@
       </c>
       <c r="H19" s="0" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -871,16 +898,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -1270,6 +1294,29 @@
       </c>
       <c r="H19" s="0" t="n">
         <v>3</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1293,16 +1340,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -1692,6 +1736,29 @@
       </c>
       <c r="H19" s="0" t="n">
         <v>20</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1715,16 +1782,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -2114,6 +2178,29 @@
       </c>
       <c r="H19" s="0" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -2137,16 +2224,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="38.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -2536,6 +2620,29 @@
       </c>
       <c r="H19" s="0" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2559,16 +2666,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -2958,6 +3062,29 @@
       </c>
       <c r="H19" s="0" t="n">
         <v>14</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -2981,16 +3108,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -3380,6 +3504,29 @@
       </c>
       <c r="H19" s="0" t="n">
         <v>19</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -3403,16 +3550,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -3802,6 +3946,29 @@
       </c>
       <c r="H19" s="0" t="n">
         <v>3</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -3825,17 +3992,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T19"/>
+  <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="13" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.780612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.4132653061224"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4395,9 +4560,9 @@
       <c r="N17" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="O17" s="0" t="e">
+      <c r="O17" s="0" t="n">
         <f aca="false">DEVSQ(robot_anticipate!$J$8:$J$17,robot_anticipate!$K$8:$K$17)</f>
-        <v>#VALUE!</v>
+        <v>10.1055555555555</v>
       </c>
       <c r="P17" s="0" t="n">
         <f aca="false">SUM(robot_anticipate!$O$11:$O$12) - 1</f>
@@ -4448,6 +4613,29 @@
       </c>
       <c r="H19" s="0" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -4471,16 +4659,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S19"/>
+  <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -5062,9 +5247,9 @@
       <c r="M18" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="N18" s="0" t="e">
+      <c r="N18" s="0" t="n">
         <f aca="false">DEVSQ(robot_asExpected!$J$8:$J$17,robot_asExpected!$K$8:$K$17)</f>
-        <v>#VALUE!</v>
+        <v>14.3111111111111</v>
       </c>
       <c r="O18" s="0" t="n">
         <f aca="false">SUM(robot_asExpected!$N$12:$N$13) - 1</f>
@@ -5092,6 +5277,29 @@
       </c>
       <c r="H19" s="0" t="n">
         <v>5</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -5115,16 +5323,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S19"/>
+  <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -5683,9 +5888,9 @@
       <c r="M17" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="N17" s="0" t="e">
+      <c r="N17" s="0" t="n">
         <f aca="false">DEVSQ(robot_rightTiming!$J$8:$J$17,robot_rightTiming!$K$8:$K$17)</f>
-        <v>#VALUE!</v>
+        <v>13.5333333333333</v>
       </c>
       <c r="O17" s="0" t="n">
         <f aca="false">SUM(robot_rightTiming!$N$11:$N$12) - 1</f>
@@ -5736,6 +5941,29 @@
       </c>
       <c r="H19" s="0" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -5759,16 +5987,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -6169,6 +6394,29 @@
       </c>
       <c r="H19" s="0" t="n">
         <v>4</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -6192,16 +6440,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S19"/>
+  <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -6763,9 +7008,9 @@
       <c r="M17" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="N17" s="0" t="e">
+      <c r="N17" s="0" t="n">
         <f aca="false">DEVSQ(robot_moreAssistance!$J$8:$J$17,robot_moreAssistance!$K$8:$K$17)</f>
-        <v>#VALUE!</v>
+        <v>5.2222222222222</v>
       </c>
       <c r="O17" s="0" t="n">
         <f aca="false">SUM(robot_moreAssistance!$N$11:$N$12) - 1</f>
@@ -6816,6 +7061,29 @@
       </c>
       <c r="H19" s="0" t="n">
         <v>4</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -6839,16 +7107,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S19"/>
+  <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -7407,9 +7672,9 @@
       <c r="M17" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="N17" s="0" t="e">
+      <c r="N17" s="0" t="n">
         <f aca="false">DEVSQ(robot_warning!$J$8:$J$17,robot_warning!$K$8:$K$17)</f>
-        <v>#VALUE!</v>
+        <v>26.1055555555556</v>
       </c>
       <c r="O17" s="0" t="n">
         <f aca="false">SUM(robot_warning!$N$11:$N$12) - 1</f>
@@ -7459,6 +7724,29 @@
         <v>5</v>
       </c>
       <c r="H19" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H20" s="0" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7483,16 +7771,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T16"/>
+  <dimension ref="A1:T17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
+      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -7979,9 +8264,9 @@
       <c r="N14" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="O14" s="0" t="e">
+      <c r="O14" s="0" t="n">
         <f aca="false">DEVSQ(robot_repetitive!$K$5:$K$14,robot_repetitive!$L$5:$L$14)</f>
-        <v>#VALUE!</v>
+        <v>22.9777777777778</v>
       </c>
       <c r="P14" s="0" t="n">
         <f aca="false">SUM(robot_repetitive!$O$8:$O$9) - 1</f>
@@ -8032,6 +8317,29 @@
       </c>
       <c r="H16" s="9" t="n">
         <v>5</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -8055,16 +8363,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T19"/>
+  <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -8623,9 +8928,9 @@
       <c r="N17" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="O17" s="0" t="e">
+      <c r="O17" s="0" t="n">
         <f aca="false">DEVSQ(robot_notWant!$K$8:$K$17,robot_notWant!$L$8:$L$17)</f>
-        <v>#VALUE!</v>
+        <v>17.9111111111111</v>
       </c>
       <c r="P17" s="0" t="n">
         <f aca="false">SUM(robot_notWant!$O$11:$O$12) - 1</f>
@@ -8676,6 +8981,29 @@
       </c>
       <c r="H19" s="0" t="n">
         <v>5</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -8699,16 +9027,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T19"/>
+  <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -9270,9 +9595,9 @@
       <c r="N17" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="O17" s="0" t="e">
+      <c r="O17" s="0" t="n">
         <f aca="false">DEVSQ(robot_trust!$K$8:$K$17,robot_trust!$L$8:$L$17)</f>
-        <v>#VALUE!</v>
+        <v>14.1055555555556</v>
       </c>
       <c r="P17" s="0" t="n">
         <f aca="false">SUM(robot_trust!$O$11:$O$12) - 1</f>
@@ -9323,6 +9648,29 @@
       </c>
       <c r="H19" s="0" t="n">
         <v>5</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -9346,16 +9694,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T19"/>
+  <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -9914,9 +10259,9 @@
       <c r="N17" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="O17" s="0" t="e">
+      <c r="O17" s="0" t="n">
         <f aca="false">DEVSQ(robot_competitive!$K$8:$K$17,robot_competitive!$L$8:$L$17)</f>
-        <v>#VALUE!</v>
+        <v>33.6166666666667</v>
       </c>
       <c r="P17" s="0" t="n">
         <f aca="false">SUM(robot_competitive!$O$11:$O$12) - 1</f>
@@ -9967,6 +10312,29 @@
       </c>
       <c r="H19" s="0" t="n">
         <v>5</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -9990,23 +10358,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
@@ -10182,6 +10550,17 @@
       </c>
       <c r="C18" s="0" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -10203,23 +10582,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
@@ -10395,6 +10774,17 @@
       </c>
       <c r="C18" s="0" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -10416,23 +10806,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
@@ -10608,6 +10998,17 @@
       </c>
       <c r="C18" s="0" t="n">
         <v>5</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -10629,23 +11030,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
@@ -10821,6 +11222,17 @@
       </c>
       <c r="C18" s="0" t="n">
         <v>5</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -10842,16 +11254,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -11251,6 +11660,29 @@
         <v>4</v>
       </c>
       <c r="H19" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H20" s="0" t="n">
         <v>4</v>
       </c>
     </row>
@@ -11275,23 +11707,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
@@ -11467,6 +11899,17 @@
       </c>
       <c r="C18" s="0" t="n">
         <v>5</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -11488,23 +11931,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
@@ -11776,9 +12219,9 @@
       <c r="F15" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="G15" s="0" t="e">
+      <c r="G15" s="0" t="n">
         <f aca="false">DEVSQ(g_robot_adaptation!$B$7:$B$16,g_robot_adaptation!$C$7:$C$16)</f>
-        <v>#VALUE!</v>
+        <v>18.55</v>
       </c>
       <c r="H15" s="0" t="n">
         <f aca="false">SUM(g_robot_adaptation!$G$9:$G$10) - 1</f>
@@ -11816,6 +12259,17 @@
       </c>
       <c r="C18" s="0" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -11837,23 +12291,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
@@ -12136,9 +12590,9 @@
       <c r="F16" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="G16" s="0" t="e">
+      <c r="G16" s="0" t="n">
         <f aca="false">DEVSQ(g_robot_workWith!$B$7:$B$16,g_robot_workWith!$C$7:$C$16)</f>
-        <v>#VALUE!</v>
+        <v>21.8</v>
       </c>
       <c r="H16" s="0" t="n">
         <f aca="false">SUM(g_robot_workWith!$G$10:$G$11) - 1</f>
@@ -12164,6 +12618,17 @@
         <v>5</v>
       </c>
       <c r="C18" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C19" s="0" t="n">
         <v>4</v>
       </c>
     </row>
@@ -12186,23 +12651,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
@@ -12488,9 +12953,9 @@
       <c r="F16" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="G16" s="0" t="e">
+      <c r="G16" s="0" t="n">
         <f aca="false">DEVSQ(g_robot_interest!$B$7:$B$16,g_robot_interest!$C$7:$C$16)</f>
-        <v>#VALUE!</v>
+        <v>20.95</v>
       </c>
       <c r="H16" s="0" t="n">
         <f aca="false">SUM(g_robot_interest!$G$10:$G$11) - 1</f>
@@ -12517,6 +12982,17 @@
       </c>
       <c r="C18" s="0" t="n">
         <v>5</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -12538,23 +13014,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
@@ -12840,9 +13316,9 @@
       <c r="F16" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="G16" s="0" t="e">
+      <c r="G16" s="0" t="n">
         <f aca="false">DEVSQ(g_robot_like!$B$7:$B$16,g_robot_like!$C$7:$C$16)</f>
-        <v>#VALUE!</v>
+        <v>14.95</v>
       </c>
       <c r="H16" s="0" t="n">
         <f aca="false">SUM(g_robot_like!$G$10:$G$11) - 1</f>
@@ -12869,6 +13345,17 @@
       </c>
       <c r="C18" s="0" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -12890,23 +13377,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L36" activeCellId="0" sqref="L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
@@ -13192,9 +13679,9 @@
       <c r="F16" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="G16" s="0" t="e">
+      <c r="G16" s="0" t="n">
         <f aca="false">DEVSQ(g_robot_comfortable!$B$7:$B$16,g_robot_comfortable!$C$7:$C$16)</f>
-        <v>#VALUE!</v>
+        <v>15.8</v>
       </c>
       <c r="H16" s="0" t="n">
         <f aca="false">SUM(g_robot_comfortable!$G$10:$G$11) - 1</f>
@@ -13221,6 +13708,17 @@
       </c>
       <c r="C18" s="0" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -13242,23 +13740,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
+      <selection pane="topLeft" activeCell="J38" activeCellId="0" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="46.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
       <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
@@ -13287,7 +13785,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>72</v>
@@ -13317,7 +13815,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13365,7 +13863,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13381,6 +13879,14 @@
         <v>15</v>
       </c>
       <c r="B15" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>70</v>
       </c>
     </row>
@@ -13403,23 +13909,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L21" activeCellId="0" sqref="L21"/>
+      <selection pane="topLeft" activeCell="I41" activeCellId="0" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
       <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
@@ -13450,11 +13956,11 @@
       <c r="B4" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="11" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E4" s="11" t="n">
-        <v>0.1</v>
+      <c r="D4" s="12" t="n">
+        <v>0.2308</v>
+      </c>
+      <c r="E4" s="12" t="n">
+        <v>0.7692</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13470,7 +13976,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13526,7 +14032,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13542,6 +14048,14 @@
         <v>15</v>
       </c>
       <c r="B15" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>69</v>
       </c>
     </row>
@@ -13564,16 +14078,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -13962,6 +14473,29 @@
         <v>1</v>
       </c>
       <c r="H19" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" s="0" t="n">
         <v>2</v>
       </c>
     </row>
@@ -13986,16 +14520,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -14385,6 +14916,29 @@
       </c>
       <c r="H19" s="0" t="n">
         <v>4</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -14408,16 +14962,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+      <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -14807,6 +15358,29 @@
       </c>
       <c r="H19" s="0" t="n">
         <v>5</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -14830,18 +15404,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
         <v>15</v>
       </c>
@@ -15228,6 +15799,29 @@
         <v>3</v>
       </c>
       <c r="H19" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H20" s="0" t="n">
         <v>2</v>
       </c>
     </row>
@@ -15252,16 +15846,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -15651,6 +16242,29 @@
       </c>
       <c r="H19" s="0" t="n">
         <v>5</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -15674,16 +16288,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -16073,6 +16684,29 @@
       </c>
       <c r="H19" s="0" t="n">
         <v>5</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
part-17 results are analysed and added
</commit_message>
<xml_diff>
--- a/code/results/userStudies_exp1_results/analysis_subjective.xlsx
+++ b/code/results/userStudies_exp1_results/analysis_subjective.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="995" firstSheet="0" activeTab="35"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="35"/>
   </bookViews>
   <sheets>
     <sheet name="task_tedious" sheetId="1" state="visible" r:id="rId2"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="75">
   <si>
     <t xml:space="preserve">The tasks were tedious (boring and monotonous)</t>
   </si>
@@ -274,10 +274,10 @@
     <t xml:space="preserve">Selection</t>
   </si>
   <si>
-    <t xml:space="preserve">%30.77</t>
+    <t xml:space="preserve">%28.57</t>
   </si>
   <si>
-    <t xml:space="preserve">%69.23</t>
+    <t xml:space="preserve">%71.43</t>
   </si>
   <si>
     <t xml:space="preserve">Which robot was learning and adapting better to your assistance needs?</t>
@@ -445,13 +445,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
+      <selection pane="topLeft" activeCell="H22" activeCellId="0" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -875,6 +878,29 @@
       </c>
       <c r="H20" s="0" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -898,13 +924,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
+      <selection pane="topLeft" activeCell="K23" activeCellId="0" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -1317,6 +1346,29 @@
       </c>
       <c r="H20" s="0" t="n">
         <v>4</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1340,13 +1392,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
+      <selection pane="topLeft" activeCell="Q34" activeCellId="0" sqref="Q34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -1759,6 +1814,29 @@
       </c>
       <c r="H20" s="0" t="n">
         <v>16</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1782,13 +1860,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
+      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -2201,6 +2282,29 @@
       </c>
       <c r="H20" s="0" t="n">
         <v>5</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -2224,13 +2328,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
+      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="38.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -2643,6 +2750,29 @@
       </c>
       <c r="H20" s="0" t="n">
         <v>10</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2666,15 +2796,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
+      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="38.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
         <v>22</v>
       </c>
@@ -3084,6 +3217,29 @@
         <v>16</v>
       </c>
       <c r="H20" s="0" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H21" s="0" t="n">
         <v>17</v>
       </c>
     </row>
@@ -3108,15 +3264,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
+      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="41.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
@@ -3527,6 +3686,29 @@
       </c>
       <c r="H20" s="0" t="n">
         <v>7</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -3550,13 +3732,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
+      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -3969,6 +4154,29 @@
       </c>
       <c r="H20" s="0" t="n">
         <v>6</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -3992,15 +4200,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
+      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="13" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4636,6 +4846,29 @@
       </c>
       <c r="H20" s="0" t="n">
         <v>3</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -4659,13 +4892,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S20"/>
+  <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
+      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -5300,6 +5536,29 @@
       </c>
       <c r="H20" s="0" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -5323,13 +5582,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S20"/>
+  <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
+      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -5964,6 +6226,29 @@
       </c>
       <c r="H20" s="0" t="n">
         <v>4</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -5987,13 +6272,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
+      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -6417,6 +6705,29 @@
       </c>
       <c r="H20" s="0" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -6440,13 +6751,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S20"/>
+  <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -7084,6 +7398,29 @@
       </c>
       <c r="H20" s="0" t="n">
         <v>3</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -7107,13 +7444,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S20"/>
+  <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
+      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -7748,6 +8088,29 @@
       </c>
       <c r="H20" s="0" t="n">
         <v>5</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -7771,13 +8134,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T17"/>
+  <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
+      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -8340,6 +8706,29 @@
       </c>
       <c r="H17" s="0" t="n">
         <v>3</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -8363,13 +8752,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:T21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -9003,6 +9395,29 @@
         <v>3</v>
       </c>
       <c r="H20" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H21" s="0" t="n">
         <v>2</v>
       </c>
     </row>
@@ -9027,13 +9442,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
+      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -9670,6 +10088,29 @@
         <v>4</v>
       </c>
       <c r="H20" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H21" s="0" t="n">
         <v>4</v>
       </c>
     </row>
@@ -9694,13 +10135,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
+      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -10334,6 +10778,29 @@
         <v>3</v>
       </c>
       <c r="H20" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H21" s="0" t="n">
         <v>4</v>
       </c>
     </row>
@@ -10358,16 +10825,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="11" t="s">
@@ -10561,6 +11025,17 @@
       </c>
       <c r="C19" s="0" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -10582,16 +11057,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="11" t="s">
@@ -10784,6 +11256,17 @@
         <v>4</v>
       </c>
       <c r="C19" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C20" s="0" t="n">
         <v>4</v>
       </c>
     </row>
@@ -10806,16 +11289,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="11" t="s">
@@ -11009,6 +11489,17 @@
       </c>
       <c r="C19" s="0" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -11030,16 +11521,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="11" t="s">
@@ -11233,6 +11721,17 @@
       </c>
       <c r="C19" s="0" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -11254,13 +11753,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
+      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -11684,6 +12186,29 @@
       </c>
       <c r="H20" s="0" t="n">
         <v>4</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -11707,16 +12232,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="11" t="s">
@@ -11910,6 +12432,17 @@
       </c>
       <c r="C19" s="0" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -11931,16 +12464,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="11" t="s">
@@ -12269,6 +12799,17 @@
         <v>5</v>
       </c>
       <c r="C19" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C20" s="0" t="n">
         <v>4</v>
       </c>
     </row>
@@ -12291,16 +12832,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="11" t="s">
@@ -12629,6 +13167,17 @@
         <v>4</v>
       </c>
       <c r="C19" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C20" s="0" t="n">
         <v>4</v>
       </c>
     </row>
@@ -12651,16 +13200,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="11" t="s">
@@ -12993,6 +13539,17 @@
       </c>
       <c r="C19" s="0" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -13014,16 +13571,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="11" t="s">
@@ -13356,6 +13910,17 @@
       </c>
       <c r="C19" s="0" t="n">
         <v>4</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -13377,16 +13942,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L36" activeCellId="0" sqref="L36"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H23" activeCellId="0" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="11" t="s">
@@ -13718,6 +14280,17 @@
         <v>5</v>
       </c>
       <c r="C19" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C20" s="0" t="n">
         <v>3</v>
       </c>
     </row>
@@ -13740,16 +14313,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J38" activeCellId="0" sqref="J38"/>
+      <selection pane="topLeft" activeCell="R20" activeCellId="0" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="46.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="11" t="s">
@@ -13887,6 +14457,14 @@
         <v>16</v>
       </c>
       <c r="B16" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>70</v>
       </c>
     </row>
@@ -13909,16 +14487,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I41" activeCellId="0" sqref="I41"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
@@ -13957,10 +14532,10 @@
         <v>69</v>
       </c>
       <c r="D4" s="12" t="n">
-        <v>0.2308</v>
+        <v>0.2143</v>
       </c>
       <c r="E4" s="12" t="n">
-        <v>0.7692</v>
+        <v>0.7857</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14056,6 +14631,14 @@
         <v>16</v>
       </c>
       <c r="B16" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>69</v>
       </c>
     </row>
@@ -14078,13 +14661,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
+      <selection pane="topLeft" activeCell="L26" activeCellId="0" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -14497,6 +15083,29 @@
       </c>
       <c r="H20" s="0" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -14520,13 +15129,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
+      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -14939,6 +15551,29 @@
       </c>
       <c r="H20" s="0" t="n">
         <v>3</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -14962,13 +15597,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
+      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -15381,6 +16019,29 @@
       </c>
       <c r="H20" s="0" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -15404,13 +16065,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
+      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -15823,6 +16487,29 @@
       </c>
       <c r="H20" s="0" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -15846,13 +16533,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
+      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -16265,6 +16955,29 @@
       </c>
       <c r="H20" s="0" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -16288,13 +17001,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
+      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -16706,6 +17422,29 @@
         <v>2</v>
       </c>
       <c r="H20" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H21" s="0" t="n">
         <v>2</v>
       </c>
     </row>

</xml_diff>